<commit_message>
Updated to sync Item No and Mfr Catalog No if one is missing
</commit_message>
<xml_diff>
--- a/results/SouthernHospitality_Full.xlsx
+++ b/results/SouthernHospitality_Full.xlsx
@@ -528,12 +528,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HS20</t>
+          <t>HS12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HS12</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -543,12 +543,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.southernhospitality.co.nz/media/catalog/product/cache/9f6a41c099c087d3ca52f820da12388c/H/S/HS20-6490443dd4c70_1.jpg</t>
+          <t>https://www.southernhospitality.co.nz/media/catalog/product/cache/9f6a41c099c087d3ca52f820da12388c/H/S/HS12-66306af095817_1.jpg</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>HS20-6490443dd4c70_1.jpg</t>
+          <t>HS12-66306af095817_1.jpg</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -573,12 +573,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Silikomart 8 Cavity Silicone Mould Stone 85</t>
+          <t>Silikomart 5 Cup Silicone Muffin Pan</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Shipped from Supplier</t>
+          <t>In Stock</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>$56.82</t>
+          <t>$36.65</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -603,43 +603,39 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Baking Accessories</t>
+          <t>Kitchenware</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Moulds &amp; Cutters</t>
+          <t>Pastry Items</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>The Silikomart 8 Cavity Silicone Mould Stone 85 is designed to create rounded individual portions that are as visually appealing as they are delicious. Crafted with a special border, this exceptional silicone mould elevates your culinary creations to new heights. The Stone 85 exemplifies the highest standards of quality and craftsmanship. Its heat resistance ranges from -60°C to 230°C, allowing you to explore a wide range of creative possibilities with confidence. This mould is not only versatile but also dishwasher safe, making cleanup a breeze in your busy bakery, café, patisserie, or professional kitchen. Each cavity has a volume of 85ml, enabling you to create elegant and consistent individual portions in bulk. The total volume of 680ml ensures efficient production, saving you valuable time without compromising on quality or presentation.
-Whether you're a master baker, a café owner, or a pastry chef, the Silikomart 8 Cavity Silicone Mould Stone 85 is your ideal partner. Embrace the possibilities offered by this versatile tool and captivate your customers with impeccably shaped, rounded portions that are as delightful to the eyes as they are to the taste buds.
-Features
-Classic Design: The Stone 85 mould features a timeless and elegant design, allowing you to create rounded individual portions that add a touch of sophistication to your culinary creations.
-Special Border: With a unique border design, this mould ensures perfectly shaped and defined portions, enhancing the visual appeal of your dishes.
-Made in Italy: Crafted with precision and attention to detail, the Stone 85 is proudly made in Italy, guaranteeing exceptional quality and craftsmanship.
-Heat Resistance: This mould is heat resistant in a wide temperature range, from -60°C to 230°C, making it suitable for various baking, freezing, and moulding applications.
-Dishwasher Safe: Designed for convenience, the Stone 85 is dishwasher safe, allowing for easy and effortless cleaning, saving you valuable time and effort.
-Cavity Volume: Each cavity of the Stone 85 mould has a volume of 85ml, allowing you to create portions that are visually pleasing and consistent in size.
-Total Volume: The total volume of 680ml ensures efficient production, enabling you to cater to high-demand environments such as bakeries, cafés, and patisseries.
-Versatile Applications: The Stone 85 mould can be used to create a wide variety of individual desserts, pastries, mousses, and more, giving you the freedom to unleash your creativity.
-Durable and Long-lasting: Constructed from high-quality silicone, the Stone 85 mould is built to withstand frequent use and maintain its performance over time, ensuring a lasting investment for your business.
-Dimensions: 180mm x 335mm x 30mm (WxLxH) and a diameter of 65mm.</t>
+          <t>This silicone muffin pan is designed for professional and commercial baking. With a heat resistance range from -60°C to 230°C, it ensures durability and flexibility for various baking applications. Ideal for bakeries, cafés, patisseries, and more.
+Feature
+Wide Temperature Range:
+Withstands -60°C to 230°C, suitable for freezing and baking.
+Non-Stick Surface:
+Naturally non-stick
+Durable &amp; Flexible:
+Maintains its shape while allowing easy removal of muffins.
+Dishwasher Safe:
+Ensures quick and convenient cleaning.
+Versatile Use:
+Perfect for bakeries, cafés, patisseries, and other commercial kitchens.
+Specifications:
+Dimensions:
+81mm x 35mm
+Material:
+Silicone</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>HS19</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
           <t>Silikomart</t>
@@ -647,12 +643,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.southernhospitality.co.nz/media/catalog/product/cache/9f6a41c099c087d3ca52f820da12388c/H/S/HS19-648b006cd78d6_1.jpg</t>
+          <t>https://www.southernhospitality.co.nz/media/catalog/product/cache/9f6a41c099c087d3ca52f820da12388c/H/S/HS2HX-61677cfbb792d_1.jpg</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>HS19-648b006cd78d6_1.jpg</t>
+          <t>HS2HX-61677cfbb792d_1.jpg</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -677,14 +673,10 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Silikomart 8 Cavity Silicone Mould Gem 100</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Shipped from Supplier</t>
-        </is>
-      </c>
+          <t>Silikomart Fibreglass Non-Stick Mat</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -697,7 +689,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>$56.82</t>
+          <t>$43.21</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -707,206 +699,15 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Baking Accessories</t>
+          <t>Kitchenware</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Moulds &amp; Cutters</t>
+          <t>Pastry Items</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
-        <is>
-          <t>The Silikomart 8 Cavity Silicone Mould Gem 100 revolutionizes the creation of mono portions with a generous volume of 100ml. Designed with a simple and harmonious style, this exceptional silicone mould enables you to craft exquisite culinary creations with ease. Crafted in Italy with utmost precision, the GEM 100 surpasses expectations with its exceptional features. From extreme temperatures of -60°C to a scorching 230°C, this mould remains resilient, allowing you to explore a wide range of culinary possibilities. Its heat resistance ensures consistent results every time, while its dishwasher-safe quality guarantees effortless cleaning, freeing up valuable time for your bakery, café, patisserie, or any professional kitchen.
-The GEM 100 boasts 8 perfectly sized cavities, each accommodating a volume of 100ml. The total volume of 800ml ensures efficiency and productivity, allowing you to streamline your production process without compromising on quality. Whether you're an artisanal baker, a coffee shop owner, or a pastry chef, the Silikomart 8 Cavity Silicone Mould Gem 100 is your ideal companion.
-Features
-Premium Quality: Made in Italy, this mould exemplifies excellence in craftsmanship and is built to withstand the rigours of professional kitchens.
-Heat Resistance: The GEM 100 is heat resistant in a wide temperature range, from -60°C to 230°C. This allows for versatile applications, including baking, freezing, and moulding various ingredients.
-Dishwasher Safe: Designed for convenience, this silicone mould is dishwasher safe, making cleanup quick and effortless.
-8 Cavities: With 8 perfectly sized cavities, each capable of holding 100ml, this mould enables efficient production of mono portions, saving time and resources.
-Generous Total Volume: The total volume of 800ml ensures productivity and scalability, making it suitable for high-demand environments such as bakeries, cafés, and patisseries.
-Versatile Applications: The GEM 100 can be used to create a wide variety of culinary delights, from individual desserts and pastries to savoury dishes and artistic food presentations.
-Easy Release: The flexible silicone material and precise design of the mould allow for easy release of your creations without compromising their shape or texture.
-Durable and Long-lasting: Constructed from high-quality silicone, the GEM 100 is built to endure frequent use and maintain its performance over time.
-Professional-Grade: Silikomart Professional is a trusted brand in the culinary industry, known for providing top-notch products that meet the demanding standards of professional chefs and bakers.
-Dimensions: 61mm x 61mm x 30mm (LxWxH)</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Silikomart</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>https://www.southernhospitality.co.nz/media/catalog/product/cache/9f6a41c099c087d3ca52f820da12388c/H/S/HS16HX-62fa370b85285_1.jpg</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>HS16HX-62fa370b85285_1.jpg</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Silikomart AirMat Microperforated Mat</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>$46.30</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>Kitchenware &amp; Barware</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>Baking Accessories</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Pans &amp; Trays</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>The Silikomart AirMat is a Microperforated silicone mat with a fibreglass core. Perfect for baking éclairs, cookies, cream puffs, petits-fours, bread and pizza. The holes in the mat allow the heat to spread evenly throughout the mats’ surfaces, allowing for even baking. These Silikomart AirMats can also be used for additional support when freezing due to their non-slip and non-stick features.
-Features
-Usable across a temperature range from – 60°C  + 230°C.
-Can be cleaned in the dishwasher
-It can be taken from the oven/microwave and placed immediately in the fridge freezer and vice versa.
-If bent, the mat will regain its shape.
-Materials used to conform with EU standards
-All materials used are tested in accordance with the Foods Standards Agency.
-Avaiable in sizes:
-300mmW x 400mmH
-520mmW x 315mmH
-583mmW x 384mmH</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Silikomart</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>https://www.southernhospitality.co.nz/media/catalog/product/cache/9f6a41c099c087d3ca52f820da12388c/H/S/HS2HX-61677cfbb792d_1.jpg</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>HS2HX-61677cfbb792d_1.jpg</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Silikomart Fibreglass Non-Stick Mat</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>$43.21</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Kitchenware &amp; Barware</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Kitchenware</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>Pastry Items</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
         <is>
           <t>The Silikomart Fibreglass Non-Stick Mat takes your culinary creations to the next level. This fibreglass silicone product is designed to withstand high temperatures, prevent oxidation of metal pans, and enhance the overall appearance of your baked goods. Perfect for baking pastries, doughs, and bread, and working with sugar. This mat ensures consistent results and easy release for your baked creations.
 Features
@@ -925,13 +726,204 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>HS19</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>HS19</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Silikomart</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://www.southernhospitality.co.nz/media/catalog/product/cache/9f6a41c099c087d3ca52f820da12388c/H/S/HS19-648b006cd78d6_1.jpg</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>HS19-648b006cd78d6_1.jpg</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Silikomart 8 Cavity Silicone Mould Gem 100</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Shipped from Supplier</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>$56.82</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Kitchenware &amp; Barware</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Baking Accessories</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Moulds &amp; Cutters</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>The Silikomart 8 Cavity Silicone Mould Gem 100 revolutionizes the creation of mono portions with a generous volume of 100ml. Designed with a simple and harmonious style, this exceptional silicone mould enables you to craft exquisite culinary creations with ease. Crafted in Italy with utmost precision, the GEM 100 surpasses expectations with its exceptional features. From extreme temperatures of -60°C to a scorching 230°C, this mould remains resilient, allowing you to explore a wide range of culinary possibilities. Its heat resistance ensures consistent results every time, while its dishwasher-safe quality guarantees effortless cleaning, freeing up valuable time for your bakery, café, patisserie, or any professional kitchen.
+The GEM 100 boasts 8 perfectly sized cavities, each accommodating a volume of 100ml. The total volume of 800ml ensures efficiency and productivity, allowing you to streamline your production process without compromising on quality. Whether you're an artisanal baker, a coffee shop owner, or a pastry chef, the Silikomart 8 Cavity Silicone Mould Gem 100 is your ideal companion.
+Features
+Premium Quality: Made in Italy, this mould exemplifies excellence in craftsmanship and is built to withstand the rigours of professional kitchens.
+Heat Resistance: The GEM 100 is heat resistant in a wide temperature range, from -60°C to 230°C. This allows for versatile applications, including baking, freezing, and moulding various ingredients.
+Dishwasher Safe: Designed for convenience, this silicone mould is dishwasher safe, making cleanup quick and effortless.
+8 Cavities: With 8 perfectly sized cavities, each capable of holding 100ml, this mould enables efficient production of mono portions, saving time and resources.
+Generous Total Volume: The total volume of 800ml ensures productivity and scalability, making it suitable for high-demand environments such as bakeries, cafés, and patisseries.
+Versatile Applications: The GEM 100 can be used to create a wide variety of culinary delights, from individual desserts and pastries to savoury dishes and artistic food presentations.
+Easy Release: The flexible silicone material and precise design of the mould allow for easy release of your creations without compromising their shape or texture.
+Durable and Long-lasting: Constructed from high-quality silicone, the GEM 100 is built to endure frequent use and maintain its performance over time.
+Professional-Grade: Silikomart Professional is a trusted brand in the culinary industry, known for providing top-notch products that meet the demanding standards of professional chefs and bakers.
+Dimensions: 61mm x 61mm x 30mm (LxWxH)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Silikomart</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://www.southernhospitality.co.nz/media/catalog/product/cache/9f6a41c099c087d3ca52f820da12388c/H/S/HS16HX-62fa370b85285_1.jpg</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>HS16HX-62fa370b85285_1.jpg</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Silikomart AirMat Microperforated Mat</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>$46.30</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Kitchenware &amp; Barware</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Baking Accessories</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Pans &amp; Trays</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>The Silikomart AirMat is a Microperforated silicone mat with a fibreglass core. Perfect for baking éclairs, cookies, cream puffs, petits-fours, bread and pizza. The holes in the mat allow the heat to spread evenly throughout the mats’ surfaces, allowing for even baking. These Silikomart AirMats can also be used for additional support when freezing due to their non-slip and non-stick features.
+Features
+Usable across a temperature range from – 60°C  + 230°C.
+Can be cleaned in the dishwasher
+It can be taken from the oven/microwave and placed immediately in the fridge freezer and vice versa.
+If bent, the mat will regain its shape.
+Materials used to conform with EU standards
+All materials used are tested in accordance with the Foods Standards Agency.
+Avaiable in sizes:
+300mmW x 400mmH
+520mmW x 315mmH
+583mmW x 384mmH</t>
+        </is>
+      </c>
+    </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
           <t>Silikomart</t>
@@ -1029,12 +1021,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HS12</t>
+          <t>HS20</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HS20</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1044,12 +1036,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.southernhospitality.co.nz/media/catalog/product/cache/9f6a41c099c087d3ca52f820da12388c/H/S/HS12-66306af095817_1.jpg</t>
+          <t>https://www.southernhospitality.co.nz/media/catalog/product/cache/9f6a41c099c087d3ca52f820da12388c/H/S/HS20-6490443dd4c70_1.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>HS12-66306af095817_1.jpg</t>
+          <t>HS20-6490443dd4c70_1.jpg</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1074,12 +1066,12 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Silikomart 5 Cup Silicone Muffin Pan</t>
+          <t>Silikomart 8 Cavity Silicone Mould Stone 85</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>In Stock</t>
+          <t>Shipped from Supplier</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -1094,7 +1086,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>$36.65</t>
+          <t>$56.82</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -1104,33 +1096,29 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Kitchenware</t>
+          <t>Baking Accessories</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Pastry Items</t>
+          <t>Moulds &amp; Cutters</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>This silicone muffin pan is designed for professional and commercial baking. With a heat resistance range from -60°C to 230°C, it ensures durability and flexibility for various baking applications. Ideal for bakeries, cafés, patisseries, and more.
-Feature
-Wide Temperature Range:
-Withstands -60°C to 230°C, suitable for freezing and baking.
-Non-Stick Surface:
-Naturally non-stick
-Durable &amp; Flexible:
-Maintains its shape while allowing easy removal of muffins.
-Dishwasher Safe:
-Ensures quick and convenient cleaning.
-Versatile Use:
-Perfect for bakeries, cafés, patisseries, and other commercial kitchens.
-Specifications:
-Dimensions:
-81mm x 35mm
-Material:
-Silicone</t>
+          <t>The Silikomart 8 Cavity Silicone Mould Stone 85 is designed to create rounded individual portions that are as visually appealing as they are delicious. Crafted with a special border, this exceptional silicone mould elevates your culinary creations to new heights. The Stone 85 exemplifies the highest standards of quality and craftsmanship. Its heat resistance ranges from -60°C to 230°C, allowing you to explore a wide range of creative possibilities with confidence. This mould is not only versatile but also dishwasher safe, making cleanup a breeze in your busy bakery, café, patisserie, or professional kitchen. Each cavity has a volume of 85ml, enabling you to create elegant and consistent individual portions in bulk. The total volume of 680ml ensures efficient production, saving you valuable time without compromising on quality or presentation.
+Whether you're a master baker, a café owner, or a pastry chef, the Silikomart 8 Cavity Silicone Mould Stone 85 is your ideal partner. Embrace the possibilities offered by this versatile tool and captivate your customers with impeccably shaped, rounded portions that are as delightful to the eyes as they are to the taste buds.
+Features
+Classic Design: The Stone 85 mould features a timeless and elegant design, allowing you to create rounded individual portions that add a touch of sophistication to your culinary creations.
+Special Border: With a unique border design, this mould ensures perfectly shaped and defined portions, enhancing the visual appeal of your dishes.
+Made in Italy: Crafted with precision and attention to detail, the Stone 85 is proudly made in Italy, guaranteeing exceptional quality and craftsmanship.
+Heat Resistance: This mould is heat resistant in a wide temperature range, from -60°C to 230°C, making it suitable for various baking, freezing, and moulding applications.
+Dishwasher Safe: Designed for convenience, the Stone 85 is dishwasher safe, allowing for easy and effortless cleaning, saving you valuable time and effort.
+Cavity Volume: Each cavity of the Stone 85 mould has a volume of 85ml, allowing you to create portions that are visually pleasing and consistent in size.
+Total Volume: The total volume of 680ml ensures efficient production, enabling you to cater to high-demand environments such as bakeries, cafés, and patisseries.
+Versatile Applications: The Stone 85 mould can be used to create a wide variety of individual desserts, pastries, mousses, and more, giving you the freedom to unleash your creativity.
+Durable and Long-lasting: Constructed from high-quality silicone, the Stone 85 mould is built to withstand frequent use and maintain its performance over time, ensuring a lasting investment for your business.
+Dimensions: 180mm x 335mm x 30mm (WxLxH) and a diameter of 65mm.</t>
         </is>
       </c>
     </row>

</xml_diff>